<commit_message>
Generate Fix Message handler and order execution
</commit_message>
<xml_diff>
--- a/src/main/resources/StoryAndTask.xlsx
+++ b/src/main/resources/StoryAndTask.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijayshreejoshi/Documents/java/mobileapplication/database sem 2/Dissertation/submition/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijayshreejoshi/Documents/java/mobileapplication/database sem 2/Dissertation/submition/code/middlewareapp/fixengine/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E19AE23-1489-0D48-8FF6-A178889A7E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9A7DE1-9F4B-B64F-B110-2D02C7A15A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DAE2A747-0696-DF48-AE19-0E5F99ABEFA3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{DAE2A747-0696-DF48-AE19-0E5F99ABEFA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>User Story</t>
   </si>
@@ -163,6 +163,24 @@
   </si>
   <si>
     <t xml:space="preserve">S6T1: </t>
+  </si>
+  <si>
+    <t>S8: As a user I want  accept order functinality so that I can accept the executed order.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S9: As a user I want execute order functionality so that user can execute order </t>
+  </si>
+  <si>
+    <t>S7: As a user I want to enhance login functinality so that user can login as trader or broker role</t>
+  </si>
+  <si>
+    <t>S10: As a user I want logout functinality.</t>
+  </si>
+  <si>
+    <t>S7T1: As a developer I need to add radio buttons for trader and broker so that user can able to select one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S7T2: As a developer I need to </t>
   </si>
 </sst>
 </file>
@@ -549,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEC3E26-1A18-B644-A509-2C64CAC8AE11}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -775,6 +793,34 @@
         <v>38</v>
       </c>
     </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B14:B15"/>

</xml_diff>

<commit_message>
code quality and improvement
</commit_message>
<xml_diff>
--- a/src/main/resources/StoryAndTask.xlsx
+++ b/src/main/resources/StoryAndTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijayshreejoshi/Documents/java/mobileapplication/database sem 2/Dissertation/submition/code/middlewareapp/fixengine/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DADE02A-FF5C-3F43-BBF7-24FF9258FB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE8C4AE-C7D4-584F-A2C2-F93994154628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{DAE2A747-0696-DF48-AE19-0E5F99ABEFA3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>User Story</t>
   </si>
@@ -156,9 +156,6 @@
     <t>S6: Aa user I want to see portfolio of all client.</t>
   </si>
   <si>
-    <t xml:space="preserve">S6T1: </t>
-  </si>
-  <si>
     <t>S8: As a user I want  accept order functinality so that I can accept the executed order.</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t xml:space="preserve">          function and same application will use by trader and broker.</t>
   </si>
   <si>
-    <t>S7T5: As a developer I need to add some finctinality on button to disbale and enble accordingly.</t>
-  </si>
-  <si>
     <t>S10T1: As a developer I need to add logout button on home page so that user will able to logout safely.</t>
   </si>
   <si>
@@ -223,6 +217,33 @@
   </si>
   <si>
     <t>S8T4: As a developer I need to create symbol table in database.</t>
+  </si>
+  <si>
+    <t>S6T1: As a developer I need to create portfolio Button in UI(Android)</t>
+  </si>
+  <si>
+    <t>S4T4: As a developer I need to add finctinily so that succesfull message will appear for user.</t>
+  </si>
+  <si>
+    <t>S6T2: As a developer I need to set on click listener in android.</t>
+  </si>
+  <si>
+    <t>S6T3: As a developer I need to create new screen to show all details of order submission.</t>
+  </si>
+  <si>
+    <t>S6T4: As a developer I need to create search bar so that user can enter account id to see particular client portfolio.</t>
+  </si>
+  <si>
+    <t>S6T5: As a developer I need to create functinality so that information retirve from database and show on UI with REST</t>
+  </si>
+  <si>
+    <t>S6T6: AS a developer I need to create</t>
+  </si>
+  <si>
+    <t>S7T5: As a developer I need to add some functionality  on button to disbale and enble accordingly.</t>
+  </si>
+  <si>
+    <t>S10T1: As a developer I need to add a message for successfully logout.</t>
   </si>
 </sst>
 </file>
@@ -612,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AEC3E26-1A18-B644-A509-2C64CAC8AE11}">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,12 +762,12 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -780,6 +801,11 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -828,7 +854,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -838,63 +864,88 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>36</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" t="s">
         <v>39</v>
-      </c>
-      <c r="B56" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B69" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B70" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -914,33 +965,38 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B85" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B87" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B89" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>